<commit_message>
27 de out as 11
</commit_message>
<xml_diff>
--- a/parceiros_inst.xlsx
+++ b/parceiros_inst.xlsx
@@ -27,25 +27,25 @@
     <t>Instituicao</t>
   </si>
   <si>
+    <t>PARQUE DE CHIMANIMANI</t>
+  </si>
+  <si>
+    <t>UCM</t>
+  </si>
+  <si>
+    <t>MICAIA</t>
+  </si>
+  <si>
+    <t>ISPM</t>
+  </si>
+  <si>
+    <t>ITAM</t>
+  </si>
+  <si>
     <t>UNIZAMBEZE</t>
   </si>
   <si>
     <t>SDAE SUSSUNDENGA</t>
-  </si>
-  <si>
-    <t>ISPM</t>
-  </si>
-  <si>
-    <t>UCM</t>
-  </si>
-  <si>
-    <t>MICAIA</t>
-  </si>
-  <si>
-    <t>ITAM</t>
-  </si>
-  <si>
-    <t>PARQUE DE CHIMANIMANI</t>
   </si>
   <si>
     <t>PARQUE DE GORONGOSA</t>
@@ -129,10 +129,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0">
         <v>1</v>
@@ -163,13 +163,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -180,10 +180,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0">
         <v>1</v>
@@ -197,13 +197,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -214,10 +214,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="0">
         <v>1</v>

</xml_diff>

<commit_message>
8 sessao dos homens chimanimani
</commit_message>
<xml_diff>
--- a/parceiros_inst.xlsx
+++ b/parceiros_inst.xlsx
@@ -27,25 +27,25 @@
     <t>Instituicao</t>
   </si>
   <si>
+    <t>UNIZAMBEZE</t>
+  </si>
+  <si>
+    <t>MICAIA</t>
+  </si>
+  <si>
+    <t>SDAE SUSSUNDENGA</t>
+  </si>
+  <si>
     <t>PARQUE DE CHIMANIMANI</t>
   </si>
   <si>
+    <t>ITAM</t>
+  </si>
+  <si>
     <t>ISPM</t>
   </si>
   <si>
     <t>UCM</t>
-  </si>
-  <si>
-    <t>SDAE SUSSUNDENGA</t>
-  </si>
-  <si>
-    <t>UNIZAMBEZE</t>
-  </si>
-  <si>
-    <t>MICAIA</t>
-  </si>
-  <si>
-    <t>ITAM</t>
   </si>
   <si>
     <t>PARQUE DE GORONGOSA</t>
@@ -129,10 +129,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0">
         <v>1</v>
@@ -146,13 +146,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -197,10 +197,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0">
         <v>1</v>
@@ -214,13 +214,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">

</xml_diff>